<commit_message>
DUAl-STRIDE and Jacobson scheme
</commit_message>
<xml_diff>
--- a/DUAl-STRIDE.xlsx
+++ b/DUAl-STRIDE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chiaragobbi/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://univpm-my.sharepoint.com/personal/s1109495_studenti_univpm_it/Documents/Primo Anno/Primo semestre/Software Security and Blockchain/swsb-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A6B3E1A8-3907-CF4F-B3F6-D673E0C5A57E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{A6B3E1A8-3907-CF4F-B3F6-D673E0C5A57E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EAA28FAE-5DF5-4A66-9FB0-A4CB77695782}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Policy Objectives" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="154">
   <si>
     <t>Asset</t>
   </si>
@@ -663,9 +663,6 @@
     <t>9.600-18.000</t>
   </si>
   <si>
-    <t>CI DOBBIAMO RAGIONARE</t>
-  </si>
-  <si>
     <t>300-450</t>
   </si>
   <si>
@@ -676,7 +673,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1516,6 +1513,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1821,24 +1822,24 @@
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="15" style="3" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="10.796875" style="3" customWidth="1"/>
     <col min="3" max="7" width="6.5" style="3" customWidth="1"/>
-    <col min="8" max="8" width="6.6640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="6.69921875" style="3" customWidth="1"/>
     <col min="9" max="11" width="6.5" style="3" customWidth="1"/>
-    <col min="12" max="12" width="10.83203125" style="3"/>
+    <col min="12" max="12" width="10.796875" style="3"/>
     <col min="13" max="13" width="20" style="3" customWidth="1"/>
     <col min="14" max="15" width="10" style="3" customWidth="1"/>
     <col min="16" max="16" width="20" style="3" customWidth="1"/>
     <col min="17" max="17" width="10" style="3" customWidth="1"/>
-    <col min="18" max="18" width="10.83203125" style="3"/>
+    <col min="18" max="18" width="10.796875" style="3"/>
     <col min="19" max="21" width="10" style="3" customWidth="1"/>
-    <col min="22" max="16384" width="10.83203125" style="3"/>
+    <col min="22" max="16384" width="10.796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="10" customFormat="1" ht="22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="10" customFormat="1" ht="21">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -1863,7 +1864,7 @@
       <c r="T1" s="57"/>
       <c r="U1" s="57"/>
     </row>
-    <row r="2" spans="1:21" s="10" customFormat="1" ht="22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" s="10" customFormat="1" ht="21">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1892,7 +1893,7 @@
       <c r="T2" s="57"/>
       <c r="U2" s="57"/>
     </row>
-    <row r="3" spans="1:21" s="10" customFormat="1" ht="22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" s="10" customFormat="1" ht="21">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1921,7 +1922,7 @@
       <c r="T3" s="12"/>
       <c r="U3" s="12"/>
     </row>
-    <row r="5" spans="1:21" ht="22" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" ht="21">
       <c r="A5" s="13" t="s">
         <v>0</v>
       </c>
@@ -1941,7 +1942,7 @@
       </c>
       <c r="J5" s="62"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21">
       <c r="A6" s="8"/>
       <c r="B6" s="9"/>
       <c r="C6" s="53"/>
@@ -1953,7 +1954,7 @@
       <c r="I6" s="64"/>
       <c r="J6" s="54"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21">
       <c r="A7" s="8"/>
       <c r="B7" s="9"/>
       <c r="C7" s="53"/>
@@ -1965,7 +1966,7 @@
       <c r="I7" s="64"/>
       <c r="J7" s="54"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21">
       <c r="A8" s="8"/>
       <c r="B8" s="9"/>
       <c r="C8" s="53"/>
@@ -1977,7 +1978,7 @@
       <c r="I8" s="64"/>
       <c r="J8" s="54"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21">
       <c r="A9" s="8"/>
       <c r="B9" s="9"/>
       <c r="C9" s="53"/>
@@ -1989,7 +1990,7 @@
       <c r="I9" s="64"/>
       <c r="J9" s="54"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21">
       <c r="A10" s="8"/>
       <c r="B10" s="9"/>
       <c r="C10" s="53"/>
@@ -2001,7 +2002,7 @@
       <c r="I10" s="64"/>
       <c r="J10" s="54"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21">
       <c r="A11" s="8"/>
       <c r="B11" s="9"/>
       <c r="C11" s="53"/>
@@ -2013,7 +2014,7 @@
       <c r="I11" s="64"/>
       <c r="J11" s="54"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21">
       <c r="A12" s="8"/>
       <c r="B12" s="9"/>
       <c r="C12" s="53"/>
@@ -2025,7 +2026,7 @@
       <c r="I12" s="64"/>
       <c r="J12" s="54"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21">
       <c r="A13" s="8"/>
       <c r="B13" s="9"/>
       <c r="C13" s="53"/>
@@ -2037,7 +2038,7 @@
       <c r="I13" s="64"/>
       <c r="J13" s="54"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21">
       <c r="A14" s="8"/>
       <c r="B14" s="9"/>
       <c r="C14" s="53"/>
@@ -2049,7 +2050,7 @@
       <c r="I14" s="64"/>
       <c r="J14" s="54"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21">
       <c r="A15" s="8"/>
       <c r="B15" s="9"/>
       <c r="C15" s="53"/>
@@ -2061,7 +2062,7 @@
       <c r="I15" s="64"/>
       <c r="J15" s="54"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21">
       <c r="A16" s="8"/>
       <c r="B16" s="9"/>
       <c r="C16" s="53"/>
@@ -2073,7 +2074,7 @@
       <c r="I16" s="64"/>
       <c r="J16" s="54"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10">
       <c r="A17" s="8"/>
       <c r="B17" s="9"/>
       <c r="C17" s="53"/>
@@ -2085,7 +2086,7 @@
       <c r="I17" s="64"/>
       <c r="J17" s="54"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10">
       <c r="A18" s="8"/>
       <c r="B18" s="9"/>
       <c r="C18" s="53"/>
@@ -2097,7 +2098,7 @@
       <c r="I18" s="64"/>
       <c r="J18" s="54"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10">
       <c r="A19" s="8"/>
       <c r="B19" s="9"/>
       <c r="C19" s="53"/>
@@ -2109,7 +2110,7 @@
       <c r="I19" s="64"/>
       <c r="J19" s="54"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10">
       <c r="A20" s="8"/>
       <c r="B20" s="9"/>
       <c r="C20" s="53"/>
@@ -2121,7 +2122,7 @@
       <c r="I20" s="64"/>
       <c r="J20" s="54"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10">
       <c r="A21" s="8"/>
       <c r="B21" s="9"/>
       <c r="C21" s="53"/>
@@ -2133,7 +2134,7 @@
       <c r="I21" s="64"/>
       <c r="J21" s="54"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10">
       <c r="A22" s="8"/>
       <c r="B22" s="9"/>
       <c r="C22" s="53"/>
@@ -2145,7 +2146,7 @@
       <c r="I22" s="64"/>
       <c r="J22" s="54"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10">
       <c r="A23" s="8"/>
       <c r="B23" s="9"/>
       <c r="C23" s="53"/>
@@ -2157,7 +2158,7 @@
       <c r="I23" s="64"/>
       <c r="J23" s="54"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10">
       <c r="A24" s="8"/>
       <c r="B24" s="9"/>
       <c r="C24" s="53"/>
@@ -2169,7 +2170,7 @@
       <c r="I24" s="64"/>
       <c r="J24" s="54"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10">
       <c r="A25" s="8"/>
       <c r="B25" s="9"/>
       <c r="C25" s="53"/>
@@ -2243,28 +2244,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AB42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AB21" sqref="AB21"/>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="AA7" sqref="AA7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="16.796875" style="3" customWidth="1"/>
     <col min="2" max="2" width="12.5" style="2" customWidth="1"/>
-    <col min="3" max="11" width="6.83203125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="13.83203125" style="2" customWidth="1"/>
+    <col min="3" max="11" width="6.796875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="13.796875" style="2" customWidth="1"/>
     <col min="13" max="14" width="33" style="3" customWidth="1"/>
     <col min="15" max="16" width="10" style="3" customWidth="1"/>
     <col min="17" max="17" width="20" style="3" customWidth="1"/>
     <col min="18" max="19" width="10" style="3" customWidth="1"/>
-    <col min="20" max="20" width="61.33203125" style="3" customWidth="1"/>
+    <col min="20" max="20" width="61.296875" style="3" customWidth="1"/>
     <col min="21" max="26" width="10" style="3" customWidth="1"/>
-    <col min="27" max="27" width="29.1640625" style="3" customWidth="1"/>
-    <col min="28" max="28" width="76.6640625" style="3" customWidth="1"/>
-    <col min="29" max="16384" width="10.83203125" style="3"/>
+    <col min="27" max="27" width="29.19921875" style="3" customWidth="1"/>
+    <col min="28" max="28" width="76.69921875" style="3" customWidth="1"/>
+    <col min="29" max="16384" width="10.796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="10" customFormat="1" ht="22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" s="10" customFormat="1" ht="21">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -2294,7 +2295,7 @@
       <c r="Y1" s="3"/>
       <c r="Z1" s="3"/>
     </row>
-    <row r="2" spans="1:28" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" s="10" customFormat="1" ht="25.05" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -2330,7 +2331,7 @@
       <c r="Y2" s="3"/>
       <c r="Z2" s="3"/>
     </row>
-    <row r="3" spans="1:28" s="10" customFormat="1" ht="22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" s="10" customFormat="1" ht="21">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -2364,7 +2365,7 @@
       <c r="Y3" s="41"/>
       <c r="Z3" s="12"/>
     </row>
-    <row r="4" spans="1:28" ht="157" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" ht="157.05000000000001" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
@@ -2448,7 +2449,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:28" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" ht="72" customHeight="1">
       <c r="A5" s="66" t="s">
         <v>29</v>
       </c>
@@ -2518,7 +2519,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:28" ht="71" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" ht="70.95" customHeight="1">
       <c r="A6" s="80"/>
       <c r="B6" s="80"/>
       <c r="C6" s="67"/>
@@ -2567,7 +2568,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:28" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28" ht="85.05" customHeight="1">
       <c r="A7" s="67"/>
       <c r="B7" s="67"/>
       <c r="C7" s="18" t="s">
@@ -2636,7 +2637,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28" ht="85.05" customHeight="1">
       <c r="A8" s="86" t="s">
         <v>35</v>
       </c>
@@ -2702,7 +2703,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28" ht="85.05" customHeight="1">
       <c r="A9" s="85"/>
       <c r="B9" s="85"/>
       <c r="C9" s="85"/>
@@ -2744,7 +2745,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:28" ht="85.05" customHeight="1">
       <c r="A10" s="83" t="s">
         <v>37</v>
       </c>
@@ -2804,7 +2805,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="11" spans="1:28" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:28" ht="85.05" customHeight="1">
       <c r="A11" s="84"/>
       <c r="B11" s="84"/>
       <c r="C11" s="84"/>
@@ -2846,7 +2847,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="12" spans="1:28" ht="61" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28" ht="61.05" customHeight="1">
       <c r="A12" s="66" t="s">
         <v>42</v>
       </c>
@@ -2906,7 +2907,7 @@
         <v>-0.9</v>
       </c>
     </row>
-    <row r="13" spans="1:28" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" ht="60" customHeight="1">
       <c r="A13" s="67"/>
       <c r="B13" s="70"/>
       <c r="C13" s="67"/>
@@ -2948,7 +2949,7 @@
         <v>-0.9</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28" ht="39" customHeight="1">
       <c r="A14" s="66" t="s">
         <v>30</v>
       </c>
@@ -3004,7 +3005,7 @@
         <v>-0.3</v>
       </c>
     </row>
-    <row r="15" spans="1:28" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:28" ht="39.75" customHeight="1">
       <c r="A15" s="67"/>
       <c r="B15" s="67"/>
       <c r="C15" s="67"/>
@@ -3046,7 +3047,7 @@
         <v>-0.4</v>
       </c>
     </row>
-    <row r="16" spans="1:28" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28" ht="39.75" customHeight="1">
       <c r="A16" s="66" t="s">
         <v>31</v>
       </c>
@@ -3105,7 +3106,7 @@
       </c>
       <c r="AA16" s="68"/>
     </row>
-    <row r="17" spans="1:27" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:27" ht="40.5" customHeight="1">
       <c r="A17" s="67"/>
       <c r="B17" s="67"/>
       <c r="C17" s="67"/>
@@ -3148,7 +3149,7 @@
       </c>
       <c r="AA17" s="68"/>
     </row>
-    <row r="18" spans="1:27" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:27" ht="40.5" customHeight="1">
       <c r="A18" s="66" t="s">
         <v>32</v>
       </c>
@@ -3208,7 +3209,7 @@
         <v>-0.6</v>
       </c>
     </row>
-    <row r="19" spans="1:27" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:27" ht="40.5" customHeight="1">
       <c r="A19" s="80"/>
       <c r="B19" s="80"/>
       <c r="C19" s="67"/>
@@ -3250,7 +3251,7 @@
         <v>-0.7</v>
       </c>
     </row>
-    <row r="20" spans="1:27" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:27" ht="40.5" customHeight="1">
       <c r="A20" s="66" t="s">
         <v>67</v>
       </c>
@@ -3310,7 +3311,7 @@
         <v>-0.6</v>
       </c>
     </row>
-    <row r="21" spans="1:27" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:27" ht="40.5" customHeight="1">
       <c r="A21" s="67"/>
       <c r="B21" s="67"/>
       <c r="C21" s="67"/>
@@ -3352,7 +3353,7 @@
         <v>-0.7</v>
       </c>
     </row>
-    <row r="22" spans="1:27" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:27" ht="40.5" customHeight="1">
       <c r="A22" s="66" t="s">
         <v>33</v>
       </c>
@@ -3414,7 +3415,7 @@
         <v>-0.2</v>
       </c>
     </row>
-    <row r="23" spans="1:27" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:27" ht="40.5" customHeight="1">
       <c r="A23" s="80"/>
       <c r="B23" s="80"/>
       <c r="C23" s="67"/>
@@ -3456,7 +3457,7 @@
         <v>-0.3</v>
       </c>
     </row>
-    <row r="24" spans="1:27" ht="83" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:27" ht="82.95" customHeight="1">
       <c r="A24" s="67"/>
       <c r="B24" s="67"/>
       <c r="C24" s="18"/>
@@ -3514,7 +3515,7 @@
         <v>-0.9</v>
       </c>
     </row>
-    <row r="25" spans="1:27" ht="138" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:27" ht="138" customHeight="1">
       <c r="A25" s="66" t="s">
         <v>34</v>
       </c>
@@ -3582,7 +3583,7 @@
         <v>-0.2</v>
       </c>
     </row>
-    <row r="26" spans="1:27" ht="106" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:27" ht="106.05" customHeight="1">
       <c r="A26" s="80"/>
       <c r="B26" s="80"/>
       <c r="C26" s="67"/>
@@ -3624,7 +3625,7 @@
         <v>-0.3</v>
       </c>
     </row>
-    <row r="27" spans="1:27" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:27" ht="90" customHeight="1">
       <c r="A27" s="80"/>
       <c r="B27" s="80"/>
       <c r="C27" s="66"/>
@@ -3682,7 +3683,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:27" ht="67" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:27" ht="67.05" customHeight="1">
       <c r="A28" s="80"/>
       <c r="B28" s="80"/>
       <c r="C28" s="67"/>
@@ -3730,7 +3731,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="29" spans="1:27" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:27" ht="40.5" customHeight="1">
       <c r="A29" s="67"/>
       <c r="B29" s="67"/>
       <c r="C29" s="18" t="s">
@@ -3777,11 +3778,9 @@
       <c r="X29" s="15"/>
       <c r="Y29" s="15"/>
       <c r="Z29" s="39"/>
-      <c r="AA29" s="52" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="30" spans="1:27" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AA29" s="52"/>
+    </row>
+    <row r="30" spans="1:27" ht="90" customHeight="1">
       <c r="A30" s="90" t="s">
         <v>85</v>
       </c>
@@ -3836,7 +3835,7 @@
         <v>90</v>
       </c>
       <c r="X30" s="15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Y30" s="21" t="s">
         <v>80</v>
@@ -3845,7 +3844,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="31" spans="1:27" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:27" ht="103.2" customHeight="1">
       <c r="A31" s="91"/>
       <c r="B31" s="80"/>
       <c r="C31" s="23"/>
@@ -3894,7 +3893,7 @@
         <v>50</v>
       </c>
       <c r="X31" s="15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Y31" s="25" t="s">
         <v>80</v>
@@ -3903,30 +3902,30 @@
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="1:27" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:27" ht="41.25" customHeight="1">
       <c r="Y32" s="24"/>
     </row>
-    <row r="33" spans="11:12" ht="41.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="34" spans="11:12" ht="35.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" spans="11:12" ht="65.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" spans="11:12" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="11:12" ht="41.25" customHeight="1"/>
+    <row r="34" spans="11:12" ht="35.25" customHeight="1"/>
+    <row r="36" spans="11:12" ht="65.25" customHeight="1"/>
+    <row r="37" spans="11:12" ht="65.25" customHeight="1">
       <c r="L37" s="3"/>
     </row>
-    <row r="38" spans="11:12" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="11:12" ht="65.25" customHeight="1">
       <c r="L38" s="3"/>
     </row>
-    <row r="39" spans="11:12" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="11:12" ht="65.25" customHeight="1">
       <c r="L39" s="3"/>
     </row>
-    <row r="40" spans="11:12" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="11:12" ht="65.25" customHeight="1">
       <c r="K40" s="3"/>
       <c r="L40" s="3"/>
     </row>
-    <row r="41" spans="11:12" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="11:12" ht="65.25" customHeight="1">
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
     </row>
-    <row r="42" spans="11:12" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="11:12" ht="65.25" customHeight="1">
       <c r="K42" s="3"/>
       <c r="L42" s="3"/>
     </row>
@@ -3966,6 +3965,8 @@
     <mergeCell ref="I8:I9"/>
     <mergeCell ref="J8:J9"/>
     <mergeCell ref="K8:K9"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="K14:K15"/>
     <mergeCell ref="T8:T23"/>
     <mergeCell ref="T25:T26"/>
     <mergeCell ref="Q25:Q26"/>
@@ -3990,6 +3991,10 @@
     <mergeCell ref="D18:D19"/>
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="L14:L15"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="J14:J15"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="C20:C21"/>
     <mergeCell ref="D20:D21"/>
@@ -3999,17 +4004,6 @@
     <mergeCell ref="H20:H21"/>
     <mergeCell ref="I20:I21"/>
     <mergeCell ref="J20:J21"/>
-    <mergeCell ref="K16:K17"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="J14:J15"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="D14:D15"/>
@@ -4027,6 +4021,11 @@
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="G18:G19"/>
     <mergeCell ref="F18:F19"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="G16:G17"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="M12:M13"/>
     <mergeCell ref="L12:L13"/>
@@ -4120,6 +4119,6 @@
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <pageSetup paperSize="8" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>